<commit_message>
Cards + Loans added
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\tcr-legaldocs\RPA\REPOS\RPA021_FNB_CAS_account_data_verification\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\legaldocs\RPA\REPOS\RPA021_FNB_CAS_account_data_verification\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -158,13 +158,13 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>FNB CAS Account data extraction</t>
+    <t>RPA021 Cards/Loans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -537,7 +537,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Update Process to be more dynamic
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -158,13 +158,13 @@
     <t xml:space="preserve">The maximum number of consecutive system exceptions was reached. </t>
   </si>
   <si>
-    <t>RPA021 Cards/Loans</t>
+    <t>Nutun Legal</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -586,9 +586,6 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" t="s">
-        <v>44</v>
-      </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
@@ -597,7 +594,9 @@
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>44</v>
+      </c>
       <c r="C3" s="4" t="s">
         <v>32</v>
       </c>

</xml_diff>